<commit_message>
fix: improve more components to be more reusable
</commit_message>
<xml_diff>
--- a/client/src/assets/storage/phase-one/static/similarity_scores.xlsx
+++ b/client/src/assets/storage/phase-one/static/similarity_scores.xlsx
@@ -14,12 +14,18 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="2">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="4">
   <si>
     <t>C:/Users/Hangsihak Sin/OneDrive/Documents/School/Doc-Wise/backend/phase_one/temp_files\Assignment_3_Group17.pdf</t>
   </si>
   <si>
-    <t>C:/Users/Hangsihak Sin/OneDrive/Documents/School/Doc-Wise/backend/phase_one/temp_files\CV_Canadien_anglais.pdf</t>
+    <t>C:/Users/Hangsihak Sin/OneDrive/Documents/School/Doc-Wise/backend/phase_one/temp_files\model_linkedin.docx</t>
+  </si>
+  <si>
+    <t>C:/Users/Hangsihak Sin/OneDrive/Documents/School/Doc-Wise/backend/phase_one/temp_files\net2.pdf</t>
+  </si>
+  <si>
+    <t>C:/Users/Hangsihak Sin/OneDrive/Documents/School/Doc-Wise/backend/phase_one/temp_files\Ryan-Lattrel_App-Note.pdf</t>
   </si>
 </sst>
 </file>
@@ -377,40 +383,92 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C3"/>
+  <dimension ref="A1:E5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:5">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>1</v>
       </c>
+      <c r="D1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>3</v>
+      </c>
     </row>
-    <row r="2" spans="1:3">
+    <row r="2" spans="1:5">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B2">
-        <v>0.9999999403953558</v>
+        <v>0.9999999403953554</v>
       </c>
       <c r="C2">
-        <v>0.3104400592447091</v>
+        <v>0.4689624690312765</v>
+      </c>
+      <c r="D2">
+        <v>0.5073443268135294</v>
+      </c>
+      <c r="E2">
+        <v>0.4179190944842692</v>
       </c>
     </row>
-    <row r="3" spans="1:3">
+    <row r="3" spans="1:5">
       <c r="A3" s="1" t="s">
         <v>1</v>
       </c>
       <c r="B3">
-        <v>0.3104400592447091</v>
+        <v>0.4689624690312765</v>
       </c>
       <c r="C3">
-        <v>1.000000178813935</v>
+        <v>1.000000119209291</v>
+      </c>
+      <c r="D3">
+        <v>0.4948627427259438</v>
+      </c>
+      <c r="E3">
+        <v>0.305423068565764</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5">
+      <c r="A4" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B4">
+        <v>0.5073443268135294</v>
+      </c>
+      <c r="C4">
+        <v>0.4948627427259438</v>
+      </c>
+      <c r="D4">
+        <v>0.9999999403953582</v>
+      </c>
+      <c r="E4">
+        <v>0.5091269485357147</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5">
+      <c r="A5" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B5">
+        <v>0.4179190944842692</v>
+      </c>
+      <c r="C5">
+        <v>0.305423068565764</v>
+      </c>
+      <c r="D5">
+        <v>0.5091269485357147</v>
+      </c>
+      <c r="E5">
+        <v>1.000000059604645</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
add: set up phase two interface for backend
</commit_message>
<xml_diff>
--- a/client/src/assets/storage/phase-one/static/similarity_scores.xlsx
+++ b/client/src/assets/storage/phase-one/static/similarity_scores.xlsx
@@ -16,7 +16,7 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="2">
   <si>
-    <t>C:/Users/Hangsihak Sin/OneDrive/Documents/School/Doc-Wise/backend/phase_one/temp_files\Hangsihak_Sin_Resume.docx</t>
+    <t>C:/Users/Hangsihak Sin/OneDrive/Documents/School/Doc-Wise/backend/phase_one/temp_files\net2.pdf</t>
   </si>
   <si>
     <t>C:/Users/Hangsihak Sin/OneDrive/Documents/School/Doc-Wise/backend/phase_one/temp_files\Test_Plan_Requirements.pdf</t>
@@ -396,10 +396,10 @@
         <v>0</v>
       </c>
       <c r="B2">
-        <v>0.9999999999999987</v>
+        <v>0.9999999403953509</v>
       </c>
       <c r="C2">
-        <v>0.4608543988638943</v>
+        <v>0.4796421785405556</v>
       </c>
     </row>
     <row r="3" spans="1:3">
@@ -407,10 +407,10 @@
         <v>1</v>
       </c>
       <c r="B3">
-        <v>0.4608543988638943</v>
+        <v>0.4796421785405556</v>
       </c>
       <c r="C3">
-        <v>1</v>
+        <v>0.9999999999999998</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
fix: add extra argument to handle upload to differential which phase is called
</commit_message>
<xml_diff>
--- a/client/src/assets/storage/phase-one/static/similarity_scores.xlsx
+++ b/client/src/assets/storage/phase-one/static/similarity_scores.xlsx
@@ -14,7 +14,13 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="2">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="4">
+  <si>
+    <t>C:/Users/Hangsihak Sin/OneDrive/Documents/School/Doc-Wise/backend/phase_one/temp_files\Hangsihak_Sin_CoverLetter_2.pdf</t>
+  </si>
+  <si>
+    <t>C:/Users/Hangsihak Sin/OneDrive/Documents/School/Doc-Wise/backend/phase_one/temp_files\Hangsihak_Sin_Transcript_1.pdf</t>
+  </si>
   <si>
     <t>C:/Users/Hangsihak Sin/OneDrive/Documents/School/Doc-Wise/backend/phase_one/temp_files\net2.pdf</t>
   </si>
@@ -377,40 +383,92 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C3"/>
+  <dimension ref="A1:E5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:5">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>1</v>
       </c>
+      <c r="D1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>3</v>
+      </c>
     </row>
-    <row r="2" spans="1:3">
+    <row r="2" spans="1:5">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B2">
-        <v>0.9999999403953509</v>
+        <v>0.9999999403953553</v>
       </c>
       <c r="C2">
-        <v>0.4796421785405556</v>
+        <v>0.4485565959896671</v>
+      </c>
+      <c r="D2">
+        <v>0.4427806619818045</v>
+      </c>
+      <c r="E2">
+        <v>0.431584213614177</v>
       </c>
     </row>
-    <row r="3" spans="1:3">
+    <row r="3" spans="1:5">
       <c r="A3" s="1" t="s">
         <v>1</v>
       </c>
       <c r="B3">
-        <v>0.4796421785405556</v>
+        <v>0.4485565959896671</v>
       </c>
       <c r="C3">
-        <v>0.9999999999999998</v>
+        <v>0.9999998807907116</v>
+      </c>
+      <c r="D3">
+        <v>0.392725977505771</v>
+      </c>
+      <c r="E3">
+        <v>0.3869618633737347</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5">
+      <c r="A4" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B4">
+        <v>0.4427806619818045</v>
+      </c>
+      <c r="C4">
+        <v>0.392725977505771</v>
+      </c>
+      <c r="D4">
+        <v>0.9999999403953526</v>
+      </c>
+      <c r="E4">
+        <v>0.4787833090451574</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5">
+      <c r="A5" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B5">
+        <v>0.431584213614177</v>
+      </c>
+      <c r="C5">
+        <v>0.3869618633737347</v>
+      </c>
+      <c r="D5">
+        <v>0.4787833090451574</v>
+      </c>
+      <c r="E5">
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>